<commit_message>
Updated function in Excel to handle Uppercase labels
</commit_message>
<xml_diff>
--- a/TRUDUtilsD365/Resource/TableFieldsBuilderTemplateV1.xlsx
+++ b/TRUDUtilsD365/Resource/TableFieldsBuilderTemplateV1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Field type</t>
   </si>
@@ -153,9 +153,6 @@
     <t>For field</t>
   </si>
   <si>
-    <t>=RemoveSpecial(PROPER(E62))</t>
-  </si>
-  <si>
     <t>For EDT</t>
   </si>
   <si>
@@ -163,6 +160,33 @@
   </si>
   <si>
     <t>Use the following functions to generate EDT or Field name</t>
+  </si>
+  <si>
+    <t>Function fLetter(str As String) As String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim strarr() As String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    strarr = Split(str)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim i As Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    For i = LBound(strarr) To UBound(strarr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        strarr(i) = UCase$(Left$(strarr(i), 1)) &amp; Mid$(strarr(i), 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Next i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    fLetter = Join(strarr, " ")</t>
+  </si>
+  <si>
+    <t>=RemoveSpecial(fLetter(E62))</t>
   </si>
 </sst>
 </file>
@@ -521,7 +545,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,12 +644,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>Lookup!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A95</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>Lookup!$B$1:$B$3</xm:f>
@@ -638,6 +656,12 @@
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Lookup!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A95</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -646,10 +670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +681,7 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -665,7 +689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -673,18 +697,18 @@
         <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -692,7 +716,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -700,7 +724,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -708,7 +732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -716,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -724,7 +748,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -732,7 +756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -740,7 +764,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -748,64 +772,60 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="4" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
     <row r="23" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
@@ -815,9 +835,58 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="1"/>
+      <c r="H25" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>